<commit_message>
Updated Report and Run metrics, and new script for testing select3
</commit_message>
<xml_diff>
--- a/Run Metrics & Calculations.xlsx
+++ b/Run Metrics & Calculations.xlsx
@@ -6,7 +6,10 @@
     <sheet state="visible" name="write_fixed_len_pages" sheetId="1" r:id="rId3"/>
     <sheet state="visible" name="read_fixed_len_page" sheetId="2" r:id="rId4"/>
     <sheet state="visible" name="csv2heapfile" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="select" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="csv2colstore" sheetId="4" r:id="rId6"/>
+    <sheet state="visible" name="select" sheetId="5" r:id="rId7"/>
+    <sheet state="visible" name="select2" sheetId="6" r:id="rId8"/>
+    <sheet state="visible" name="select3" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="29">
   <si>
     <t>Records</t>
   </si>
@@ -254,11 +257,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1444733989"/>
-        <c:axId val="636316455"/>
+        <c:axId val="1556398689"/>
+        <c:axId val="1532458298"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1444733989"/>
+        <c:axId val="1556398689"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -273,10 +276,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636316455"/>
+        <c:crossAx val="1532458298"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="636316455"/>
+        <c:axId val="1532458298"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -324,7 +327,1076 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1444733989"/>
+        <c:crossAx val="1556398689"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>select2!$C$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4684EE"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0"/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>select2!$B$13:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select2!$C$13:$C$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="280230388"/>
+        <c:axId val="1683225596"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="280230388"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Block Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1683225596"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1683225596"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Average A - D (MS)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="280230388"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>select2!$D$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4684EE"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0"/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>select2!$B$13:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select2!$D$13:$D$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1262580682"/>
+        <c:axId val="452006928"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1262580682"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Block Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="452006928"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="452006928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Average A - D (MS)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1262580682"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>select2!$E$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4684EE"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0"/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>select2!$B$13:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select2!$E$13:$E$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="991458765"/>
+        <c:axId val="1852105026"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="991458765"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Block Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1852105026"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1852105026"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="991458765"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>select3!$C$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4684EE"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0"/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>select3!$B$13:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select3!$C$13:$C$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="1457160772"/>
+        <c:axId val="921882395"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1457160772"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Block Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="921882395"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="921882395"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Average A - D (MS)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1457160772"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4684EE"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0"/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>select3!$B$12:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select3!$D$12:$D$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="1176091303"/>
+        <c:axId val="2048866846"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1176091303"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Horizontal axis title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2048866846"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2048866846"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Left vertical axis title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1176091303"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4684EE"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" i="0"/>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>select3!$B$12:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select3!$E$12:$E$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="383512056"/>
+        <c:axId val="1494782089"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="383512056"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Horizontal axis title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1494782089"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1494782089"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Left vertical axis title</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="383512056"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>select3!$C$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4684EE"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>select3!$B$13:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select3!$C$13:$C$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>select3!$D$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>select3!$B$13:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select3!$D$13:$D$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>select3!$E$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="FF9900"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>select3!$B$13:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select3!$E$13:$E$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="255774831"/>
+        <c:axId val="371186171"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="255774831"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Block Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="371186171"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="371186171"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="255774831"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -394,11 +1466,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1184363278"/>
-        <c:axId val="1714618061"/>
+        <c:axId val="556884813"/>
+        <c:axId val="1379299404"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1184363278"/>
+        <c:axId val="556884813"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -413,10 +1485,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1714618061"/>
+        <c:crossAx val="1379299404"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1714618061"/>
+        <c:axId val="1379299404"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -447,7 +1519,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1184363278"/>
+        <c:crossAx val="556884813"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -512,11 +1584,11 @@
           </c:val>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="1350614775"/>
-        <c:axId val="1887037520"/>
+        <c:axId val="1444195312"/>
+        <c:axId val="2104616634"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1350614775"/>
+        <c:axId val="1444195312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -531,10 +1603,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1887037520"/>
+        <c:crossAx val="2104616634"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1887037520"/>
+        <c:axId val="2104616634"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -565,7 +1637,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1350614775"/>
+        <c:crossAx val="1444195312"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -578,6 +1650,141 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" sz="1600">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:t>Records per second (csv2colstore)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4684EE"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>csv2colstore!$B$1:$B$10</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>csv2colstore!$H$1:$H$10</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="269777869"/>
+        <c:axId val="1712549722"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="269777869"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Page size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1712549722"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1712549722"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="269777869"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:plotArea>
@@ -673,11 +1880,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1186268422"/>
-        <c:axId val="1934101940"/>
+        <c:axId val="1098503462"/>
+        <c:axId val="11840594"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1186268422"/>
+        <c:axId val="1098503462"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -709,10 +1916,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1934101940"/>
+        <c:crossAx val="11840594"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1934101940"/>
+        <c:axId val="11840594"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -743,7 +1950,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1186268422"/>
+        <c:crossAx val="1098503462"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -755,7 +1962,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:plotArea>
@@ -809,11 +2016,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1291942836"/>
-        <c:axId val="1061070857"/>
+        <c:axId val="1368861433"/>
+        <c:axId val="1461054104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1291942836"/>
+        <c:axId val="1368861433"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -845,10 +2052,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1061070857"/>
+        <c:crossAx val="1461054104"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1061070857"/>
+        <c:axId val="1461054104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,7 +2103,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1291942836"/>
+        <c:crossAx val="1368861433"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -908,7 +2115,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:plotArea>
@@ -962,11 +2169,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="850391541"/>
-        <c:axId val="991572190"/>
+        <c:axId val="779671484"/>
+        <c:axId val="2089926305"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="850391541"/>
+        <c:axId val="779671484"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -998,10 +2205,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="991572190"/>
+        <c:crossAx val="2089926305"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="991572190"/>
+        <c:axId val="2089926305"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +2256,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="850391541"/>
+        <c:crossAx val="779671484"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1061,7 +2268,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
   <c:chart>
     <c:plotArea>
@@ -1115,11 +2322,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="534498730"/>
-        <c:axId val="1592202489"/>
+        <c:axId val="1732892808"/>
+        <c:axId val="1204760987"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="534498730"/>
+        <c:axId val="1732892808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1151,10 +2358,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1592202489"/>
+        <c:crossAx val="1204760987"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1592202489"/>
+        <c:axId val="1204760987"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1185,7 +2392,185 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="534498730"/>
+        <c:crossAx val="1732892808"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>select2!$C$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="4684EE"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>select2!$B$13:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select2!$C$13:$C$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>select2!$D$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="DC3912"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>select2!$B$13:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select2!$D$13:$D$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>select2!$E$12</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="25400">
+              <a:solidFill>
+                <a:srgbClr val="FF9900"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>select2!$B$13:$B$21</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>select2!$E$13:$E$21</c:f>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1419827945"/>
+        <c:axId val="643590009"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1419827945"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Block Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="643590009"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="643590009"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="47625">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1419827945"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -1272,13 +2657,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>933450</xdr:colOff>
+      <xdr:colOff>942975</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>876300</xdr:colOff>
+      <xdr:colOff>885825</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
@@ -1306,6 +2691,41 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/worksheetdrawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1143000</xdr:colOff>
       <xdr:row>21</xdr:row>
@@ -1319,7 +2739,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 4" title="Chart"/>
+        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1349,7 +2769,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 5" title="Chart"/>
+        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1379,7 +2799,7 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 6" title="Chart"/>
+        <xdr:cNvPr id="7" name="Chart 7" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1409,7 +2829,257 @@
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 7" title="Chart"/>
+        <xdr:cNvPr id="8" name="Chart 8" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/worksheetdrawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 9" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 10" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 11" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 12" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/worksheetdrawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="13" name="Chart 13" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 14" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 15" title="Chart"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="16" name="Chart 16" title="Chart"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2400,6 +4070,305 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>153.857</v>
+      </c>
+      <c r="D2" s="3">
+        <v>150.158</v>
+      </c>
+      <c r="E2" s="3">
+        <v>141.851</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F10" si="1">AVERAGE(C1,D2,E2)</f>
+        <v>146.0045</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G10" si="2">F2/1000</f>
+        <v>0.1460045</v>
+      </c>
+      <c r="H2" s="5" t="str">
+        <f t="shared" ref="H2:H10" si="3">A2/G2</f>
+        <v>6,849.10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3">
+        <v>136.196</v>
+      </c>
+      <c r="D3" s="3">
+        <v>138.138</v>
+      </c>
+      <c r="E3" s="3">
+        <v>145.206</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="1"/>
+        <v>145.7336667</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>0.1457336667</v>
+      </c>
+      <c r="H3" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>6,861.83</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>139.245</v>
+      </c>
+      <c r="D4" s="3">
+        <v>140.42</v>
+      </c>
+      <c r="E4" s="3">
+        <v>140.369</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="1"/>
+        <v>138.995</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>0.138995</v>
+      </c>
+      <c r="H4" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>7,194.50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>146.077</v>
+      </c>
+      <c r="D5" s="3">
+        <v>143.965</v>
+      </c>
+      <c r="E5" s="3">
+        <v>151.889</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="1"/>
+        <v>145.033</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>0.145033</v>
+      </c>
+      <c r="H5" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>6,894.98</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>140.615</v>
+      </c>
+      <c r="D6" s="3">
+        <v>142.265</v>
+      </c>
+      <c r="E6" s="3">
+        <v>137.889</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="1"/>
+        <v>142.077</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>0.142077</v>
+      </c>
+      <c r="H6" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>7,038.44</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3">
+        <v>153.719</v>
+      </c>
+      <c r="D7" s="3">
+        <v>163.461</v>
+      </c>
+      <c r="E7" s="3">
+        <v>146.661</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="1"/>
+        <v>150.2456667</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>0.1502456667</v>
+      </c>
+      <c r="H7" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>6,655.77</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3">
+        <v>157.766</v>
+      </c>
+      <c r="D8" s="3">
+        <v>174.855</v>
+      </c>
+      <c r="E8" s="3">
+        <v>154.679</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>161.0843333</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>0.1610843333</v>
+      </c>
+      <c r="H8" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>6,207.93</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3">
+        <v>198.148</v>
+      </c>
+      <c r="D9" s="3">
+        <v>227.168</v>
+      </c>
+      <c r="E9" s="3">
+        <v>199.666</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="1"/>
+        <v>194.8666667</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>0.1948666667</v>
+      </c>
+      <c r="H9" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>5,131.71</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3">
+        <v>257.465</v>
+      </c>
+      <c r="D10" s="3">
+        <v>280.582</v>
+      </c>
+      <c r="E10" s="3">
+        <v>260.768</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="1"/>
+        <v>246.4993333</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>0.2464993333</v>
+      </c>
+      <c r="H10" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>4,056.81</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="3" max="3" width="20.86"/>
     <col customWidth="1" min="4" max="6" width="22.86"/>
@@ -2935,4 +4904,1087 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="20.86"/>
+    <col customWidth="1" min="4" max="6" width="22.86"/>
+    <col customWidth="1" min="7" max="7" width="24.0"/>
+    <col customWidth="1" min="8" max="8" width="20.0"/>
+    <col customWidth="1" min="9" max="9" width="18.86"/>
+    <col customWidth="1" min="10" max="10" width="21.14"/>
+    <col customWidth="1" min="11" max="11" width="19.57"/>
+    <col customWidth="1" min="14" max="14" width="27.0"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.628</v>
+      </c>
+      <c r="D2" s="3">
+        <v>2.166</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.304</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.599</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.838</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.268</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.675</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2.323</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.385</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.81</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.237</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.397</v>
+      </c>
+      <c r="G3" s="3">
+        <v>1.874</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.231</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.393</v>
+      </c>
+      <c r="J3" s="3">
+        <v>1.786</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.251</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.364</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1.848</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.233</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.372</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.961</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.223</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="J4" s="3">
+        <v>1.785</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.242</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.362</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.048</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.241</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.498</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.316</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.261</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.415</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1.88</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.45</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1.897</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.374</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.845</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.249</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.358</v>
+      </c>
+      <c r="J6" s="3">
+        <v>1.986</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.323</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.372</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1.791</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.237</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.381</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.815</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.222</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.439</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.887</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.247</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.433</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.878</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.312</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.451</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.199</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.425</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.479</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2.045</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.342</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.872</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.178</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.655</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.21</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.573</v>
+      </c>
+      <c r="I9" s="3">
+        <v>0.872</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2.278</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.577</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.262</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.368</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.965</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.069</v>
+      </c>
+      <c r="G10" s="3">
+        <v>2.556</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1.032</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1.132</v>
+      </c>
+      <c r="J10" s="3">
+        <v>2.554</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.913</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <f t="shared" ref="C13:D13" si="1">AVERAGE(C2,F2,I2)</f>
+        <v>0.63</v>
+      </c>
+      <c r="D13" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>2.11</v>
+      </c>
+      <c r="E13" s="5" t="str">
+        <f t="shared" ref="E13:E21" si="3">AVERAGE(E2, H2, K2)</f>
+        <v>0.29</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f t="shared" ref="C14:D14" si="2">AVERAGE(C3,F3,I3)</f>
+        <v>0.39</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>1.82</v>
+      </c>
+      <c r="E14" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f t="shared" ref="C15:D15" si="4">AVERAGE(C4,F4,I4)</f>
+        <v>0.37</v>
+      </c>
+      <c r="D15" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>1.86</v>
+      </c>
+      <c r="E15" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.23</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5" t="str">
+        <f t="shared" ref="C16:D16" si="5">AVERAGE(C5,F5,I5)</f>
+        <v>0.43</v>
+      </c>
+      <c r="D16" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>2.08</v>
+      </c>
+      <c r="E16" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f t="shared" ref="C17:D17" si="6">AVERAGE(C6,F6,I6)</f>
+        <v>0.39</v>
+      </c>
+      <c r="D17" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>1.91</v>
+      </c>
+      <c r="E17" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.26</v>
+      </c>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18">
+      <c r="B18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f t="shared" ref="C18:D18" si="7">AVERAGE(C7,F7,I7)</f>
+        <v>0.40</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>1.83</v>
+      </c>
+      <c r="E18" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <f t="shared" ref="C19:D19" si="8">AVERAGE(C8,F8,I8)</f>
+        <v>0.45</v>
+      </c>
+      <c r="D19" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>2.04</v>
+      </c>
+      <c r="E19" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="5" t="str">
+        <f t="shared" ref="C20:D20" si="9">AVERAGE(C9,F9,I9)</f>
+        <v>0.83</v>
+      </c>
+      <c r="D20" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>2.22</v>
+      </c>
+      <c r="E20" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.60</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <f t="shared" ref="C21:D21" si="10">AVERAGE(C10,F10,I10)</f>
+        <v>1.15</v>
+      </c>
+      <c r="D21" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>2.49</v>
+      </c>
+      <c r="E21" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.97</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="19.43"/>
+    <col customWidth="1" min="4" max="4" width="26.57"/>
+    <col customWidth="1" min="5" max="5" width="20.71"/>
+    <col customWidth="1" min="6" max="6" width="21.57"/>
+    <col customWidth="1" min="7" max="7" width="20.14"/>
+    <col customWidth="1" min="8" max="8" width="20.43"/>
+    <col customWidth="1" min="9" max="9" width="20.57"/>
+    <col customWidth="1" min="10" max="10" width="21.29"/>
+    <col customWidth="1" min="11" max="11" width="23.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.994</v>
+      </c>
+      <c r="D2" s="3">
+        <v>3.595</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1.088</v>
+      </c>
+      <c r="F2" s="3">
+        <v>0.943</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3.45</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.888</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.946</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2.766</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.657</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.561</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2.444</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.489</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.651</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2.622</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.389</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.627</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2.179</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.378</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.529</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2.036</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.369</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.509</v>
+      </c>
+      <c r="G4" s="3">
+        <v>2.049</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.532</v>
+      </c>
+      <c r="I4" s="3">
+        <v>0.614</v>
+      </c>
+      <c r="J4" s="3">
+        <v>2.486</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.365</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.601</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.038</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.432</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.524</v>
+      </c>
+      <c r="G5" s="3">
+        <v>2.123</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.371</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.489</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2.642</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.425</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.172</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.36</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.502</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2.003</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.388</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.492</v>
+      </c>
+      <c r="J6" s="3">
+        <v>2.071</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.727</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.466</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.446</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.568</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2.123</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.389</v>
+      </c>
+      <c r="I7" s="3">
+        <v>0.499</v>
+      </c>
+      <c r="J7" s="3">
+        <v>2.644</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.425</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.622</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.85</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.531</v>
+      </c>
+      <c r="F8" s="3">
+        <v>0.757</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.233</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.517</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.737</v>
+      </c>
+      <c r="J8" s="3">
+        <v>2.326</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.472</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.694</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.945</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.1</v>
+      </c>
+      <c r="G9" s="3">
+        <v>2.66</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.945</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.271</v>
+      </c>
+      <c r="J9" s="3">
+        <v>2.706</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>1000.0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2.181</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3.351</v>
+      </c>
+      <c r="E10" s="3">
+        <v>1.475</v>
+      </c>
+      <c r="F10" s="3">
+        <v>1.82</v>
+      </c>
+      <c r="G10" s="3">
+        <v>4.245</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1.535</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1.626</v>
+      </c>
+      <c r="J10" s="3">
+        <v>3.314</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5" t="str">
+        <f t="shared" ref="C13:D13" si="1">AVERAGE(C2,F2,I2)</f>
+        <v>0.96</v>
+      </c>
+      <c r="D13" s="5" t="str">
+        <f t="shared" si="1"/>
+        <v>3.27</v>
+      </c>
+      <c r="E13" s="5" t="str">
+        <f t="shared" ref="E13:E21" si="3">AVERAGE(E2, H2, K2)</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5" t="str">
+        <f t="shared" ref="C14:D14" si="2">AVERAGE(C3,F3,I3)</f>
+        <v>0.61</v>
+      </c>
+      <c r="D14" s="5" t="str">
+        <f t="shared" si="2"/>
+        <v>2.42</v>
+      </c>
+      <c r="E14" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5" t="str">
+        <f t="shared" ref="C15:D15" si="4">AVERAGE(C4,F4,I4)</f>
+        <v>0.55</v>
+      </c>
+      <c r="D15" s="5" t="str">
+        <f t="shared" si="4"/>
+        <v>2.19</v>
+      </c>
+      <c r="E15" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5" t="str">
+        <f t="shared" ref="C16:D16" si="5">AVERAGE(C5,F5,I5)</f>
+        <v>0.54</v>
+      </c>
+      <c r="D16" s="5" t="str">
+        <f t="shared" si="5"/>
+        <v>2.27</v>
+      </c>
+      <c r="E16" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="5" t="str">
+        <f t="shared" ref="C17:D17" si="6">AVERAGE(C6,F6,I6)</f>
+        <v>0.53</v>
+      </c>
+      <c r="D17" s="5" t="str">
+        <f t="shared" si="6"/>
+        <v>2.08</v>
+      </c>
+      <c r="E17" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="5" t="str">
+        <f t="shared" ref="C18:D18" si="7">AVERAGE(C7,F7,I7)</f>
+        <v>0.60</v>
+      </c>
+      <c r="D18" s="5" t="str">
+        <f t="shared" si="7"/>
+        <v>2.41</v>
+      </c>
+      <c r="E18" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="5" t="str">
+        <f t="shared" ref="C19:D19" si="8">AVERAGE(C8,F8,I8)</f>
+        <v>0.71</v>
+      </c>
+      <c r="D19" s="5" t="str">
+        <f t="shared" si="8"/>
+        <v>2.47</v>
+      </c>
+      <c r="E19" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="5" t="str">
+        <f t="shared" ref="C20:D20" si="9">AVERAGE(C9,F9,I9)</f>
+        <v>1.28</v>
+      </c>
+      <c r="D20" s="5" t="str">
+        <f t="shared" si="9"/>
+        <v>2.69</v>
+      </c>
+      <c r="E20" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="5" t="str">
+        <f t="shared" ref="C21:D21" si="10">AVERAGE(C10,F10,I10)</f>
+        <v>1.88</v>
+      </c>
+      <c r="D21" s="5" t="str">
+        <f t="shared" si="10"/>
+        <v>3.64</v>
+      </c>
+      <c r="E21" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>1.51</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>